<commit_message>
atualização do diario de bordo e do projeto quiron
</commit_message>
<xml_diff>
--- a/Doc/DIÁRIO DE BORDO.xlsx
+++ b/Doc/DIÁRIO DE BORDO.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\franc\Sistema de Informação\PROJETO-ESTÁGIO\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\quiron\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08EC0A58-8DB6-4902-B5F0-BA837B34D91C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BB1BA6F-E426-4E6B-93BE-833E5D24F22C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{DC1535F1-911C-4F3D-B97C-3A0DCDC7A6F1}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
   <si>
     <t>ENTRADA</t>
   </si>
@@ -73,6 +73,33 @@
   </si>
   <si>
     <t>DIÁRIO DE BORDO - PROJETO/ESTÁGIO</t>
+  </si>
+  <si>
+    <t>Tentativa de instalação. Erro encontrado: tabela com tamanho grande. Solução: diminuir o tamanho do VARCHAR e alterar o tipo para TEXT quando for necessário.</t>
+  </si>
+  <si>
+    <t>Instalação do java 8 (pc Renata) e instalação do sistema (foi colocado o xampp para iniciar automaticamente junto com o SO)</t>
+  </si>
+  <si>
+    <t>Consertando pdf (troca do iReport para o iText)</t>
+  </si>
+  <si>
+    <t>Reunião com o professor Leonardo e visita a enfermaria</t>
+  </si>
+  <si>
+    <t>Consertando pdf (troca do iReport para o iText) e edição ícone (photoshop)</t>
+  </si>
+  <si>
+    <t>Edição do ícone (photoshop)</t>
+  </si>
+  <si>
+    <t>PDF com o iText e finalização da edição do ícone (photoshop)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PDF com o iText </t>
+  </si>
+  <si>
+    <t>PDF com o iText e mudança de ícone de cada frame</t>
   </si>
 </sst>
 </file>
@@ -235,17 +262,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -586,10 +620,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DED794C8-B405-45CB-A522-30832FCEF4A3}">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -599,44 +633,45 @@
     <col min="3" max="3" width="15.5703125" customWidth="1"/>
     <col min="4" max="4" width="17.28515625" customWidth="1"/>
     <col min="5" max="5" width="15.28515625" customWidth="1"/>
-    <col min="6" max="6" width="10.140625" customWidth="1"/>
-    <col min="8" max="8" width="63.140625" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" style="6" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" style="6"/>
+    <col min="8" max="8" width="68.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="11"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="14"/>
     </row>
     <row r="2" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4" t="s">
+      <c r="C2" s="8"/>
+      <c r="D2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="4"/>
-      <c r="F2" s="7" t="s">
+      <c r="E2" s="8"/>
+      <c r="F2" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="8"/>
-      <c r="H2" s="12" t="s">
+      <c r="G2" s="11"/>
+      <c r="H2" s="15" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="4"/>
+      <c r="A3" s="8"/>
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
@@ -649,31 +684,33 @@
       <c r="E3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="G3" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="13"/>
+      <c r="H3" s="16"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>43787</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3">
         <v>0.58333333333333337</v>
       </c>
-      <c r="C4" s="3">
+      <c r="E4" s="3">
         <v>0.66666666666666663</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="6">
         <v>2</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="6">
         <v>2</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="H4" s="4" t="s">
         <v>9</v>
       </c>
     </row>
@@ -681,19 +718,21 @@
       <c r="A5" s="2">
         <v>43789</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3">
         <v>0.625</v>
       </c>
-      <c r="C5" s="3">
+      <c r="E5" s="3">
         <v>0.70833333333333337</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="6">
         <v>2</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="6">
         <v>4</v>
       </c>
-      <c r="H5" s="5" t="s">
+      <c r="H5" s="4" t="s">
         <v>10</v>
       </c>
     </row>
@@ -707,13 +746,13 @@
       <c r="C6" s="3">
         <v>0.5</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="6">
         <v>3</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="6">
         <v>7</v>
       </c>
-      <c r="H6" s="5" t="s">
+      <c r="H6" s="4" t="s">
         <v>11</v>
       </c>
     </row>
@@ -721,20 +760,270 @@
       <c r="A7" s="2">
         <v>43803</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3">
         <v>0.54166666666666663</v>
       </c>
-      <c r="C7" s="3">
+      <c r="E7" s="3">
         <v>0.70833333333333337</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="6">
         <v>4</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="6">
         <v>11</v>
       </c>
-      <c r="H7" s="5" t="s">
+      <c r="H7" s="4" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>43810</v>
+      </c>
+      <c r="D8" s="3">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="E8" s="3">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="F8" s="6">
+        <v>4</v>
+      </c>
+      <c r="G8" s="6">
+        <v>15</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>43811</v>
+      </c>
+      <c r="B9" s="3">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="C9" s="3">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D9" s="3">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="E9" s="3">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="F9" s="6">
+        <v>6</v>
+      </c>
+      <c r="G9" s="6">
+        <v>21</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>43878</v>
+      </c>
+      <c r="B10" s="3">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="C10" s="3">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D10" s="3">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="E10" s="3">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="F10" s="6">
+        <v>4</v>
+      </c>
+      <c r="G10" s="6">
+        <v>25</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>43879</v>
+      </c>
+      <c r="B11" s="3">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="C11" s="3">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="D11" s="3">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="E11" s="3">
+        <v>0.95833333333333337</v>
+      </c>
+      <c r="F11" s="6">
+        <v>6</v>
+      </c>
+      <c r="G11" s="6">
+        <v>31</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>43880</v>
+      </c>
+      <c r="B12" s="3">
+        <v>0.625</v>
+      </c>
+      <c r="C12" s="3">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="D12" s="3">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="E12" s="3">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="F12" s="6">
+        <v>4</v>
+      </c>
+      <c r="G12" s="6">
+        <v>35</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>43881</v>
+      </c>
+      <c r="B13" s="3">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="C13" s="3">
+        <v>0.625</v>
+      </c>
+      <c r="F13" s="6">
+        <v>2</v>
+      </c>
+      <c r="G13" s="6">
+        <v>37</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>43883</v>
+      </c>
+      <c r="B14" s="3">
+        <v>0.625</v>
+      </c>
+      <c r="C14" s="3">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="F14" s="6">
+        <v>4</v>
+      </c>
+      <c r="G14" s="6">
+        <v>41</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <v>43885</v>
+      </c>
+      <c r="B15" s="3">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="C15" s="3">
+        <v>0.75</v>
+      </c>
+      <c r="D15" s="3">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="E15" s="3">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="F15" s="6">
+        <v>6</v>
+      </c>
+      <c r="G15" s="6">
+        <v>47</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
+        <v>43886</v>
+      </c>
+      <c r="B16" s="3">
+        <v>0.625</v>
+      </c>
+      <c r="C16" s="3">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D16" s="3">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="E16" s="3">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="F16" s="6">
+        <v>3</v>
+      </c>
+      <c r="G16" s="6">
+        <v>50</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <v>43887</v>
+      </c>
+      <c r="B17" s="3">
+        <v>0.4375</v>
+      </c>
+      <c r="C17" s="3">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="D17" s="3">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="E17" s="3">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="F17" s="6">
+        <v>6</v>
+      </c>
+      <c r="G17" s="6">
+        <v>56</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G18" s="6">
+        <f>F18+G17</f>
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
identação de pdf e correção de erro nas telas de login e gerẽncia de usuários
</commit_message>
<xml_diff>
--- a/Doc/DIÁRIO DE BORDO.xlsx
+++ b/Doc/DIÁRIO DE BORDO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\quiron\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BB1BA6F-E426-4E6B-93BE-833E5D24F22C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F27A0FA-4B62-462B-AD30-A69B3158A51A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{DC1535F1-911C-4F3D-B97C-3A0DCDC7A6F1}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
   <si>
     <t>ENTRADA</t>
   </si>
@@ -100,6 +100,9 @@
   </si>
   <si>
     <t>PDF com o iText e mudança de ícone de cada frame</t>
+  </si>
+  <si>
+    <t>PDF e correção de erro na tela de login e gerência de usuário</t>
   </si>
 </sst>
 </file>
@@ -620,10 +623,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DED794C8-B405-45CB-A522-30832FCEF4A3}">
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1021,9 +1024,30 @@
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
+        <v>43888</v>
+      </c>
+      <c r="B18" s="3">
+        <v>0.3125</v>
+      </c>
+      <c r="C18" s="3">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="F18" s="6">
+        <v>2</v>
+      </c>
       <c r="G18" s="6">
         <f>F18+G17</f>
-        <v>56</v>
+        <v>58</v>
+      </c>
+      <c r="H18" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G19" s="6">
+        <f>G18+F19</f>
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
PDF Ficha de Atendimento médico e mudança de data para o formato brasileiro
</commit_message>
<xml_diff>
--- a/Doc/DIÁRIO DE BORDO.xlsx
+++ b/Doc/DIÁRIO DE BORDO.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\quiron\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F27A0FA-4B62-462B-AD30-A69B3158A51A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0207CFC5-D80B-4412-9922-B1A922E467EA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{DC1535F1-911C-4F3D-B97C-3A0DCDC7A6F1}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="26">
   <si>
     <t>ENTRADA</t>
   </si>
@@ -103,6 +103,12 @@
   </si>
   <si>
     <t>PDF e correção de erro na tela de login e gerência de usuário</t>
+  </si>
+  <si>
+    <t>PDF (correção no cartão de vacina) e pesquisa pelo nome ou data de nascimento</t>
+  </si>
+  <si>
+    <t>PDF (correção do cartão vacina e identação da anamnese)</t>
   </si>
 </sst>
 </file>
@@ -265,7 +271,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -282,6 +288,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -623,10 +630,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DED794C8-B405-45CB-A522-30832FCEF4A3}">
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -638,43 +645,43 @@
     <col min="5" max="5" width="15.28515625" customWidth="1"/>
     <col min="6" max="6" width="10.140625" style="6" customWidth="1"/>
     <col min="7" max="7" width="9.140625" style="6"/>
-    <col min="8" max="8" width="68.5703125" customWidth="1"/>
+    <col min="8" max="8" width="73.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="14"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="15"/>
     </row>
     <row r="2" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8" t="s">
+      <c r="C2" s="9"/>
+      <c r="D2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="8"/>
-      <c r="F2" s="10" t="s">
+      <c r="E2" s="9"/>
+      <c r="F2" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="11"/>
-      <c r="H2" s="15" t="s">
+      <c r="G2" s="12"/>
+      <c r="H2" s="16" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="8"/>
+      <c r="A3" s="9"/>
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
@@ -693,7 +700,7 @@
       <c r="G3" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="16"/>
+      <c r="H3" s="17"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
@@ -1031,23 +1038,77 @@
         <v>0.3125</v>
       </c>
       <c r="C18" s="3">
-        <v>0.39583333333333331</v>
+        <v>0.4375</v>
+      </c>
+      <c r="D18" s="3">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="E18" s="3">
+        <v>0.70833333333333337</v>
       </c>
       <c r="F18" s="6">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G18" s="6">
         <f>F18+G17</f>
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="H18" s="4" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
+        <v>44040</v>
+      </c>
+      <c r="B19" s="3">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="C19" s="3">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="D19" s="3">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="E19" s="3">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="F19" s="6">
+        <v>6</v>
+      </c>
       <c r="G19" s="6">
         <f>G18+F19</f>
-        <v>58</v>
+        <v>68</v>
+      </c>
+      <c r="H19" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="8">
+        <v>43890</v>
+      </c>
+      <c r="B20" s="3">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="C20" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="D20" s="3">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="E20" s="3">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="F20" s="6">
+        <v>6</v>
+      </c>
+      <c r="G20" s="6">
+        <f>G19+F20</f>
+        <v>74</v>
+      </c>
+      <c r="H20" s="4" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Quiron 2.0 (nova versão)
</commit_message>
<xml_diff>
--- a/Doc/DIÁRIO DE BORDO.xlsx
+++ b/Doc/DIÁRIO DE BORDO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\quiron\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0207CFC5-D80B-4412-9922-B1A922E467EA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40821160-9ED9-471C-87D3-F8547432D785}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{DC1535F1-911C-4F3D-B97C-3A0DCDC7A6F1}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
   <si>
     <t>ENTRADA</t>
   </si>
@@ -109,6 +109,24 @@
   </si>
   <si>
     <t>PDF (correção do cartão vacina e identação da anamnese)</t>
+  </si>
+  <si>
+    <t>Finalização do cartão de vacina e começo do PDF da ficha de atendimento</t>
+  </si>
+  <si>
+    <t>Finalização do PDF ficha de atendimento, mudança de data para formato brasileiro</t>
+  </si>
+  <si>
+    <t>Reunião com o professor Leonardo e Personalização da interface gráfica 2.0</t>
+  </si>
+  <si>
+    <t>Personalização da interface gráfica (Quiron 2.0)</t>
+  </si>
+  <si>
+    <t>Personalização da interface gráfica (Quiron 2.0) e cabeçalho em cada tela</t>
+  </si>
+  <si>
+    <t>Tentativa de criptografia e exportação do banco de dados na enfermaria</t>
   </si>
 </sst>
 </file>
@@ -630,10 +648,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DED794C8-B405-45CB-A522-30832FCEF4A3}">
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1111,6 +1129,203 @@
         <v>24</v>
       </c>
     </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
+        <v>43892</v>
+      </c>
+      <c r="B21" s="3">
+        <v>0.375</v>
+      </c>
+      <c r="C21" s="3">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="D21" s="3">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="E21" s="3">
+        <v>0.95833333333333337</v>
+      </c>
+      <c r="F21" s="6">
+        <v>6</v>
+      </c>
+      <c r="G21" s="6">
+        <f>G20+F21</f>
+        <v>80</v>
+      </c>
+      <c r="H21" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="2">
+        <v>43893</v>
+      </c>
+      <c r="B22" s="3">
+        <v>0.375</v>
+      </c>
+      <c r="C22" s="3">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="D22" s="3">
+        <v>0.625</v>
+      </c>
+      <c r="E22" s="3">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="F22" s="6">
+        <v>4</v>
+      </c>
+      <c r="G22" s="6">
+        <f t="shared" ref="G22:G27" si="0">G21+F22</f>
+        <v>84</v>
+      </c>
+      <c r="H22" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
+        <v>43895</v>
+      </c>
+      <c r="B23" s="3">
+        <v>0.375</v>
+      </c>
+      <c r="C23" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="D23" s="3">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="E23" s="3">
+        <v>0.625</v>
+      </c>
+      <c r="F23" s="6">
+        <v>5</v>
+      </c>
+      <c r="G23" s="6">
+        <f t="shared" si="0"/>
+        <v>89</v>
+      </c>
+      <c r="H23" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="2">
+        <v>43896</v>
+      </c>
+      <c r="B24" s="3">
+        <v>0.375</v>
+      </c>
+      <c r="C24" s="3">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="D24" s="3">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="E24" s="3">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="F24" s="6">
+        <v>6</v>
+      </c>
+      <c r="G24" s="6">
+        <f t="shared" si="0"/>
+        <v>95</v>
+      </c>
+      <c r="H24" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="2">
+        <v>43899</v>
+      </c>
+      <c r="B25" s="3">
+        <v>0.375</v>
+      </c>
+      <c r="C25" s="3">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="D25" s="3">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="E25" s="3">
+        <v>0.875</v>
+      </c>
+      <c r="F25" s="6">
+        <v>4</v>
+      </c>
+      <c r="G25" s="6">
+        <f t="shared" si="0"/>
+        <v>99</v>
+      </c>
+      <c r="H25" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="2">
+        <v>43900</v>
+      </c>
+      <c r="B26" s="3">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="C26" s="3">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="D26" s="3">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="E26" s="3">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="F26" s="6">
+        <v>6</v>
+      </c>
+      <c r="G26" s="6">
+        <f t="shared" si="0"/>
+        <v>105</v>
+      </c>
+      <c r="H26" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="2">
+        <v>43901</v>
+      </c>
+      <c r="B27" s="3">
+        <v>0.375</v>
+      </c>
+      <c r="C27" s="3">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="D27" s="3">
+        <v>0.625</v>
+      </c>
+      <c r="E27" s="3">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="F27" s="6">
+        <v>4</v>
+      </c>
+      <c r="G27" s="6">
+        <f t="shared" si="0"/>
+        <v>109</v>
+      </c>
+      <c r="H27" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="2">
+        <v>43902</v>
+      </c>
+      <c r="B28" s="3">
+        <v>0.39583333333333331</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="6">
     <mergeCell ref="B2:C2"/>

</xml_diff>

<commit_message>
Quiron 2.0 atualizado (criptografia, cadastro de servidores e tela inicial)
</commit_message>
<xml_diff>
--- a/Doc/DIÁRIO DE BORDO.xlsx
+++ b/Doc/DIÁRIO DE BORDO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\quiron\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40821160-9ED9-471C-87D3-F8547432D785}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3365B59-968C-41DD-8690-907B18A1DF76}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{DC1535F1-911C-4F3D-B97C-3A0DCDC7A6F1}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="36">
   <si>
     <t>ENTRADA</t>
   </si>
@@ -127,6 +127,18 @@
   </si>
   <si>
     <t>Tentativa de criptografia e exportação do banco de dados na enfermaria</t>
+  </si>
+  <si>
+    <t>Reunião com o professor Leonardo e tentativa de criptografia</t>
+  </si>
+  <si>
+    <t>Conclusão da criptografia e elaboração da página inicial</t>
+  </si>
+  <si>
+    <t>Conclusão da página inicial, ajustes no PDF e no BD e concerto de erros</t>
+  </si>
+  <si>
+    <t>Elaboração da tela de cadastro de servidores</t>
   </si>
 </sst>
 </file>
@@ -648,10 +660,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DED794C8-B405-45CB-A522-30832FCEF4A3}">
-  <dimension ref="A1:H28"/>
+  <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1323,7 +1335,100 @@
         <v>43902</v>
       </c>
       <c r="B28" s="3">
-        <v>0.39583333333333331</v>
+        <v>0.375</v>
+      </c>
+      <c r="C28" s="3">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="D28" s="3">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="E28" s="3">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="F28" s="6">
+        <v>4</v>
+      </c>
+      <c r="G28" s="6">
+        <f>G27+F28</f>
+        <v>113</v>
+      </c>
+      <c r="H28" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="2">
+        <v>43903</v>
+      </c>
+      <c r="B29" s="3">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="C29" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="D29" s="3">
+        <v>0.625</v>
+      </c>
+      <c r="E29" s="3">
+        <v>0.75</v>
+      </c>
+      <c r="F29" s="6">
+        <v>5</v>
+      </c>
+      <c r="G29" s="6">
+        <f t="shared" ref="G29:G38" si="1">G28+F29</f>
+        <v>118</v>
+      </c>
+      <c r="H29" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="2">
+        <v>43904</v>
+      </c>
+      <c r="B30" s="3">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="C30" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="D30" s="3">
+        <v>0.625</v>
+      </c>
+      <c r="E30" s="3">
+        <v>0.75</v>
+      </c>
+      <c r="F30" s="6">
+        <v>5</v>
+      </c>
+      <c r="G30" s="6">
+        <f t="shared" si="1"/>
+        <v>123</v>
+      </c>
+      <c r="H30" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="2">
+        <v>43905</v>
+      </c>
+      <c r="B31" s="3">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="C31" s="3">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="F31" s="6">
+        <v>3</v>
+      </c>
+      <c r="G31" s="6">
+        <v>126</v>
+      </c>
+      <c r="H31" s="4" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Atualização do diário de bordo
</commit_message>
<xml_diff>
--- a/Doc/DIÁRIO DE BORDO.xlsx
+++ b/Doc/DIÁRIO DE BORDO.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\quiron\Doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\franc\Documents\GitHub\quiron\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3365B59-968C-41DD-8690-907B18A1DF76}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{619CF1DC-C59D-41A1-936C-E45E8AE0DBF5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{DC1535F1-911C-4F3D-B97C-3A0DCDC7A6F1}"/>
   </bookViews>
@@ -20,18 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="44">
   <si>
     <t>ENTRADA</t>
   </si>
@@ -139,6 +133,30 @@
   </si>
   <si>
     <t>Elaboração da tela de cadastro de servidores</t>
+  </si>
+  <si>
+    <t>Tentativa de responsividade</t>
+  </si>
+  <si>
+    <t>Finalização da responsividade</t>
+  </si>
+  <si>
+    <t>Instalação e configurações - retorno</t>
+  </si>
+  <si>
+    <t>Desenvolvimento da página para o sistema</t>
+  </si>
+  <si>
+    <t>Ajustes finais e conclusão da página para o sistema</t>
+  </si>
+  <si>
+    <t>Correção de erro na criação de usuário</t>
+  </si>
+  <si>
+    <t>Reunião com o professor Leonardo</t>
+  </si>
+  <si>
+    <t>Tentativa de correção do erro na criação de usuário e reunião com o professor Leonardo</t>
   </si>
 </sst>
 </file>
@@ -660,10 +678,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DED794C8-B405-45CB-A522-30832FCEF4A3}">
-  <dimension ref="A1:H31"/>
+  <dimension ref="A1:H43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="G40" sqref="G40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -675,7 +693,7 @@
     <col min="5" max="5" width="15.28515625" customWidth="1"/>
     <col min="6" max="6" width="10.140625" style="6" customWidth="1"/>
     <col min="7" max="7" width="9.140625" style="6"/>
-    <col min="8" max="8" width="73.5703125" customWidth="1"/>
+    <col min="8" max="8" width="77.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
@@ -1377,7 +1395,7 @@
         <v>5</v>
       </c>
       <c r="G29" s="6">
-        <f t="shared" ref="G29:G38" si="1">G28+F29</f>
+        <f t="shared" ref="G29:G30" si="1">G28+F29</f>
         <v>118</v>
       </c>
       <c r="H29" s="4" t="s">
@@ -1413,13 +1431,13 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
-        <v>43905</v>
+        <v>43906</v>
       </c>
       <c r="B31" s="3">
-        <v>0.54166666666666663</v>
+        <v>0.375</v>
       </c>
       <c r="C31" s="3">
-        <v>0.66666666666666663</v>
+        <v>0.5</v>
       </c>
       <c r="F31" s="6">
         <v>3</v>
@@ -1429,6 +1447,319 @@
       </c>
       <c r="H31" s="4" t="s">
         <v>35</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="2">
+        <v>43927</v>
+      </c>
+      <c r="B32" s="3">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="C32" s="3">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D32" s="3">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="E32" s="3">
+        <v>0.875</v>
+      </c>
+      <c r="F32" s="6">
+        <v>5</v>
+      </c>
+      <c r="G32" s="6">
+        <f t="shared" ref="G32:G43" si="2">G31+F32</f>
+        <v>131</v>
+      </c>
+      <c r="H32" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="2">
+        <v>43943</v>
+      </c>
+      <c r="B33" s="3">
+        <v>0.375</v>
+      </c>
+      <c r="C33" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="D33" s="3">
+        <v>0.75</v>
+      </c>
+      <c r="E33" s="3">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="F33" s="6">
+        <v>5</v>
+      </c>
+      <c r="G33" s="6">
+        <f t="shared" si="2"/>
+        <v>136</v>
+      </c>
+      <c r="H33" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="2">
+        <v>43944</v>
+      </c>
+      <c r="B34" s="3">
+        <v>0.375</v>
+      </c>
+      <c r="C34" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="D34" s="3">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="E34" s="3">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="F34" s="6">
+        <v>5</v>
+      </c>
+      <c r="G34" s="6">
+        <f t="shared" si="2"/>
+        <v>141</v>
+      </c>
+      <c r="H34" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="2">
+        <v>43945</v>
+      </c>
+      <c r="B35" s="3">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="C35" s="3">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="D35" s="3">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="E35" s="3">
+        <v>0.875</v>
+      </c>
+      <c r="F35" s="6">
+        <v>6</v>
+      </c>
+      <c r="G35" s="6">
+        <f t="shared" si="2"/>
+        <v>147</v>
+      </c>
+      <c r="H35" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" s="2">
+        <v>44306</v>
+      </c>
+      <c r="B36" s="3">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="C36" s="3">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="D36" s="3">
+        <v>0.75</v>
+      </c>
+      <c r="E36" s="3">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="F36" s="6">
+        <v>4</v>
+      </c>
+      <c r="G36" s="6">
+        <f t="shared" si="2"/>
+        <v>151</v>
+      </c>
+      <c r="H36" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" s="2">
+        <v>44316</v>
+      </c>
+      <c r="B37" s="3">
+        <v>0.54861111111111105</v>
+      </c>
+      <c r="C37" s="3">
+        <v>0.59027777777777779</v>
+      </c>
+      <c r="D37" s="3"/>
+      <c r="E37" s="3"/>
+      <c r="F37" s="6">
+        <v>1</v>
+      </c>
+      <c r="G37" s="6">
+        <v>152</v>
+      </c>
+      <c r="H37" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" s="2">
+        <v>44319</v>
+      </c>
+      <c r="B38" s="3">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="C38" s="3">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D38" s="3">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="E38" s="3">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="F38" s="6">
+        <v>5</v>
+      </c>
+      <c r="G38" s="6">
+        <f>G37+F38</f>
+        <v>157</v>
+      </c>
+      <c r="H38" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" s="2">
+        <v>44320</v>
+      </c>
+      <c r="B39" s="3">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="C39" s="3">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="D39" s="3">
+        <v>0.75</v>
+      </c>
+      <c r="E39" s="3">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="F39" s="6">
+        <v>5</v>
+      </c>
+      <c r="G39" s="6">
+        <f>G38+F39</f>
+        <v>162</v>
+      </c>
+      <c r="H39" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" s="2">
+        <v>44321</v>
+      </c>
+      <c r="B40" s="3">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="C40" s="3">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="D40" s="3">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="E40" s="3">
+        <v>0.875</v>
+      </c>
+      <c r="F40" s="6">
+        <v>6</v>
+      </c>
+      <c r="G40" s="6">
+        <f t="shared" si="2"/>
+        <v>168</v>
+      </c>
+      <c r="H40" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" s="2">
+        <v>44322</v>
+      </c>
+      <c r="B41" s="3">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="C41" s="3">
+        <v>0.625</v>
+      </c>
+      <c r="F41" s="6">
+        <v>2</v>
+      </c>
+      <c r="G41" s="6">
+        <f t="shared" si="2"/>
+        <v>170</v>
+      </c>
+      <c r="H41" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" s="2">
+        <v>44323</v>
+      </c>
+      <c r="B42" s="3">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="C42" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="D42" s="3">
+        <v>0.54861111111111105</v>
+      </c>
+      <c r="E42" s="3">
+        <v>0.59027777777777779</v>
+      </c>
+      <c r="F42" s="6">
+        <v>3</v>
+      </c>
+      <c r="G42" s="6">
+        <f t="shared" si="2"/>
+        <v>173</v>
+      </c>
+      <c r="H42" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" s="2">
+        <v>44328</v>
+      </c>
+      <c r="B43" s="3">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="C43" s="3">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="D43" s="3">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="E43" s="3">
+        <v>0.75</v>
+      </c>
+      <c r="F43" s="6">
+        <v>5</v>
+      </c>
+      <c r="G43" s="6">
+        <f t="shared" si="2"/>
+        <v>178</v>
+      </c>
+      <c r="H43" s="4" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>